<commit_message>
support priority 'clinical trials'
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1508.14.mip_balsamic.xlsx
+++ b/tests/fixtures/orderforms/1508.14.mip_balsamic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikgrenfeldt/Documents/src/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367DCDD7-EBEF-EF4B-94DA-D9C7FDB96EDE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6BC8706-C63C-D94F-81AD-550C4AFEDE28}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1620" yWindow="460" windowWidth="27960" windowHeight="27040" tabRatio="262" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1193" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1221" uniqueCount="490">
   <si>
     <t>&lt;TABLE HEADER&gt;</t>
   </si>
@@ -1780,15 +1780,6 @@
     <t>wgs</t>
   </si>
   <si>
-    <t>twist_wgs</t>
-  </si>
-  <si>
-    <t>capture_panels</t>
-  </si>
-  <si>
-    <t>cancer_capture_panels</t>
-  </si>
-  <si>
     <t>rna</t>
   </si>
   <si>
@@ -1937,6 +1928,15 @@
   </si>
   <si>
     <t>comment</t>
+  </si>
+  <si>
+    <t>twist-wgs</t>
+  </si>
+  <si>
+    <t>capture-panels</t>
+  </si>
+  <si>
+    <t>cancer-capture-panels</t>
   </si>
 </sst>
 </file>
@@ -4637,8 +4637,8 @@
   </sheetPr>
   <dimension ref="A1:AC428"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="Z16" sqref="Z16"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -5239,7 +5239,7 @@
         <v>96</v>
       </c>
       <c r="I15" s="23" t="s">
-        <v>18</v>
+        <v>415</v>
       </c>
       <c r="J15" s="63" t="s">
         <v>94</v>
@@ -5262,10 +5262,10 @@
         <v>335</v>
       </c>
       <c r="R15" s="69" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="S15" s="70" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="T15" s="165"/>
       <c r="U15" s="33" t="s">
@@ -5286,15 +5286,15 @@
       </c>
       <c r="AA15" s="167"/>
       <c r="AB15" s="68" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="AC15" s="68" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="16" spans="1:29" s="141" customFormat="1" ht="25" customHeight="1">
       <c r="A16" s="42" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="B16" s="63" t="s">
         <v>38</v>
@@ -5318,7 +5318,7 @@
         <v>97</v>
       </c>
       <c r="I16" s="23" t="s">
-        <v>103</v>
+        <v>415</v>
       </c>
       <c r="J16" s="63" t="s">
         <v>95</v>
@@ -5361,7 +5361,7 @@
     </row>
     <row r="17" spans="1:29" s="141" customFormat="1" ht="25" customHeight="1">
       <c r="A17" s="42" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="B17" s="63" t="s">
         <v>38</v>
@@ -5385,7 +5385,7 @@
         <v>98</v>
       </c>
       <c r="I17" s="23" t="s">
-        <v>19</v>
+        <v>415</v>
       </c>
       <c r="J17" s="63" t="s">
         <v>95</v>
@@ -5426,7 +5426,7 @@
     </row>
     <row r="18" spans="1:29" s="141" customFormat="1" ht="25" customHeight="1">
       <c r="A18" s="42" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B18" s="63" t="s">
         <v>38</v>
@@ -5449,8 +5449,8 @@
       <c r="H18" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="I18" s="33" t="s">
-        <v>104</v>
+      <c r="I18" s="23" t="s">
+        <v>415</v>
       </c>
       <c r="J18" s="63" t="s">
         <v>95</v>
@@ -5491,7 +5491,7 @@
     </row>
     <row r="19" spans="1:29" s="141" customFormat="1" ht="25" customHeight="1">
       <c r="A19" s="42" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="B19" s="63" t="s">
         <v>38</v>
@@ -5514,7 +5514,7 @@
       <c r="H19" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="I19" s="197" t="s">
+      <c r="I19" s="23" t="s">
         <v>415</v>
       </c>
       <c r="J19" s="63" t="s">
@@ -5556,7 +5556,7 @@
     </row>
     <row r="20" spans="1:29" s="141" customFormat="1" ht="25" customHeight="1">
       <c r="A20" s="42" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B20" s="63" t="s">
         <v>38</v>
@@ -5579,7 +5579,7 @@
       <c r="H20" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="I20" s="197" t="s">
+      <c r="I20" s="23" t="s">
         <v>415</v>
       </c>
       <c r="J20" s="63" t="s">
@@ -5621,7 +5621,7 @@
     </row>
     <row r="21" spans="1:29" s="141" customFormat="1" ht="25" customHeight="1">
       <c r="A21" s="42" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="B21" s="63" t="s">
         <v>38</v>
@@ -5644,7 +5644,7 @@
       <c r="H21" s="23" t="s">
         <v>249</v>
       </c>
-      <c r="I21" s="197" t="s">
+      <c r="I21" s="23" t="s">
         <v>415</v>
       </c>
       <c r="J21" s="63" t="s">
@@ -5686,7 +5686,7 @@
     </row>
     <row r="22" spans="1:29" s="141" customFormat="1" ht="25" customHeight="1">
       <c r="A22" s="42" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B22" s="63" t="s">
         <v>38</v>
@@ -5709,7 +5709,7 @@
       <c r="H22" s="46" t="s">
         <v>265</v>
       </c>
-      <c r="I22" s="197" t="s">
+      <c r="I22" s="23" t="s">
         <v>415</v>
       </c>
       <c r="J22" s="63" t="s">
@@ -5751,7 +5751,7 @@
     </row>
     <row r="23" spans="1:29" ht="25" customHeight="1">
       <c r="A23" s="42" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B23" s="63" t="s">
         <v>38</v>
@@ -5774,7 +5774,7 @@
       <c r="H23" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="I23" s="197" t="s">
+      <c r="I23" s="23" t="s">
         <v>415</v>
       </c>
       <c r="J23" s="63" t="s">
@@ -5816,7 +5816,7 @@
     </row>
     <row r="24" spans="1:29" ht="25" customHeight="1">
       <c r="A24" s="42" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B24" s="63" t="s">
         <v>38</v>
@@ -5839,7 +5839,7 @@
       <c r="H24" s="197" t="s">
         <v>413</v>
       </c>
-      <c r="I24" s="197" t="s">
+      <c r="I24" s="23" t="s">
         <v>415</v>
       </c>
       <c r="J24" s="63" t="s">
@@ -5881,7 +5881,7 @@
     </row>
     <row r="25" spans="1:29" ht="25" customHeight="1">
       <c r="A25" s="42" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="B25" s="63" t="s">
         <v>38</v>
@@ -5893,7 +5893,7 @@
         <v>296</v>
       </c>
       <c r="E25" s="65" t="s">
-        <v>437</v>
+        <v>487</v>
       </c>
       <c r="F25" s="64" t="s">
         <v>78</v>
@@ -5905,7 +5905,7 @@
         <v>414</v>
       </c>
       <c r="I25" s="197" t="s">
-        <v>415</v>
+        <v>18</v>
       </c>
       <c r="J25" s="63" t="s">
         <v>95</v>
@@ -5946,7 +5946,7 @@
     </row>
     <row r="26" spans="1:29" ht="25" customHeight="1">
       <c r="A26" s="42" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="B26" s="63" t="s">
         <v>38</v>
@@ -5958,7 +5958,7 @@
         <v>258</v>
       </c>
       <c r="E26" s="65" t="s">
-        <v>437</v>
+        <v>487</v>
       </c>
       <c r="F26" s="64" t="s">
         <v>78</v>
@@ -5970,7 +5970,7 @@
         <v>414</v>
       </c>
       <c r="I26" s="197" t="s">
-        <v>415</v>
+        <v>18</v>
       </c>
       <c r="J26" s="63" t="s">
         <v>95</v>
@@ -6011,7 +6011,7 @@
     </row>
     <row r="27" spans="1:29" s="170" customFormat="1" ht="25" customHeight="1">
       <c r="A27" s="42" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B27" s="63" t="s">
         <v>38</v>
@@ -6023,7 +6023,7 @@
         <v>426</v>
       </c>
       <c r="E27" s="65" t="s">
-        <v>437</v>
+        <v>487</v>
       </c>
       <c r="F27" s="64" t="s">
         <v>78</v>
@@ -6035,7 +6035,7 @@
         <v>414</v>
       </c>
       <c r="I27" s="197" t="s">
-        <v>415</v>
+        <v>18</v>
       </c>
       <c r="J27" s="63" t="s">
         <v>95</v>
@@ -6076,7 +6076,7 @@
     </row>
     <row r="28" spans="1:29" s="170" customFormat="1" ht="25" customHeight="1">
       <c r="A28" s="42" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="B28" s="63" t="s">
         <v>38</v>
@@ -6088,7 +6088,7 @@
         <v>297</v>
       </c>
       <c r="E28" s="65" t="s">
-        <v>437</v>
+        <v>487</v>
       </c>
       <c r="F28" s="64" t="s">
         <v>78</v>
@@ -6100,7 +6100,7 @@
         <v>414</v>
       </c>
       <c r="I28" s="197" t="s">
-        <v>415</v>
+        <v>18</v>
       </c>
       <c r="J28" s="63" t="s">
         <v>95</v>
@@ -6141,7 +6141,7 @@
     </row>
     <row r="29" spans="1:29" s="170" customFormat="1" ht="25" customHeight="1">
       <c r="A29" s="42" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="B29" s="63" t="s">
         <v>38</v>
@@ -6153,7 +6153,7 @@
         <v>313</v>
       </c>
       <c r="E29" s="65" t="s">
-        <v>438</v>
+        <v>488</v>
       </c>
       <c r="F29" s="64" t="s">
         <v>78</v>
@@ -6165,7 +6165,7 @@
         <v>414</v>
       </c>
       <c r="I29" s="197" t="s">
-        <v>415</v>
+        <v>103</v>
       </c>
       <c r="J29" s="63" t="s">
         <v>95</v>
@@ -6206,7 +6206,7 @@
     </row>
     <row r="30" spans="1:29" s="170" customFormat="1" ht="25" customHeight="1">
       <c r="A30" s="42" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="B30" s="63" t="s">
         <v>38</v>
@@ -6218,7 +6218,7 @@
         <v>314</v>
       </c>
       <c r="E30" s="65" t="s">
-        <v>438</v>
+        <v>488</v>
       </c>
       <c r="F30" s="64" t="s">
         <v>78</v>
@@ -6230,7 +6230,7 @@
         <v>414</v>
       </c>
       <c r="I30" s="197" t="s">
-        <v>415</v>
+        <v>103</v>
       </c>
       <c r="J30" s="63" t="s">
         <v>95</v>
@@ -6271,7 +6271,7 @@
     </row>
     <row r="31" spans="1:29" s="170" customFormat="1" ht="25" customHeight="1">
       <c r="A31" s="42" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="B31" s="63" t="s">
         <v>38</v>
@@ -6283,7 +6283,7 @@
         <v>315</v>
       </c>
       <c r="E31" s="65" t="s">
-        <v>438</v>
+        <v>488</v>
       </c>
       <c r="F31" s="64" t="s">
         <v>78</v>
@@ -6295,7 +6295,7 @@
         <v>414</v>
       </c>
       <c r="I31" s="197" t="s">
-        <v>415</v>
+        <v>103</v>
       </c>
       <c r="J31" s="63" t="s">
         <v>95</v>
@@ -6336,7 +6336,7 @@
     </row>
     <row r="32" spans="1:29" s="170" customFormat="1" ht="25" customHeight="1">
       <c r="A32" s="42" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="B32" s="63" t="s">
         <v>38</v>
@@ -6348,7 +6348,7 @@
         <v>316</v>
       </c>
       <c r="E32" s="65" t="s">
-        <v>438</v>
+        <v>488</v>
       </c>
       <c r="F32" s="64" t="s">
         <v>78</v>
@@ -6360,7 +6360,7 @@
         <v>414</v>
       </c>
       <c r="I32" s="197" t="s">
-        <v>415</v>
+        <v>103</v>
       </c>
       <c r="J32" s="63" t="s">
         <v>95</v>
@@ -6401,7 +6401,7 @@
     </row>
     <row r="33" spans="1:29" s="170" customFormat="1" ht="25" customHeight="1">
       <c r="A33" s="42" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B33" s="63" t="s">
         <v>38</v>
@@ -6413,7 +6413,7 @@
         <v>317</v>
       </c>
       <c r="E33" s="65" t="s">
-        <v>438</v>
+        <v>488</v>
       </c>
       <c r="F33" s="64" t="s">
         <v>78</v>
@@ -6425,7 +6425,7 @@
         <v>414</v>
       </c>
       <c r="I33" s="197" t="s">
-        <v>415</v>
+        <v>103</v>
       </c>
       <c r="J33" s="63" t="s">
         <v>95</v>
@@ -6466,7 +6466,7 @@
     </row>
     <row r="34" spans="1:29" s="170" customFormat="1" ht="25" customHeight="1">
       <c r="A34" s="42" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="B34" s="63" t="s">
         <v>38</v>
@@ -6478,7 +6478,7 @@
         <v>318</v>
       </c>
       <c r="E34" s="65" t="s">
-        <v>438</v>
+        <v>488</v>
       </c>
       <c r="F34" s="64" t="s">
         <v>78</v>
@@ -6490,7 +6490,7 @@
         <v>414</v>
       </c>
       <c r="I34" s="197" t="s">
-        <v>415</v>
+        <v>103</v>
       </c>
       <c r="J34" s="63" t="s">
         <v>95</v>
@@ -6531,7 +6531,7 @@
     </row>
     <row r="35" spans="1:29" s="170" customFormat="1" ht="25" customHeight="1">
       <c r="A35" s="42" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B35" s="63" t="s">
         <v>38</v>
@@ -6543,7 +6543,7 @@
         <v>319</v>
       </c>
       <c r="E35" s="65" t="s">
-        <v>438</v>
+        <v>488</v>
       </c>
       <c r="F35" s="64" t="s">
         <v>78</v>
@@ -6555,7 +6555,7 @@
         <v>414</v>
       </c>
       <c r="I35" s="197" t="s">
-        <v>415</v>
+        <v>103</v>
       </c>
       <c r="J35" s="63" t="s">
         <v>95</v>
@@ -6594,7 +6594,7 @@
     </row>
     <row r="36" spans="1:29" s="171" customFormat="1" ht="25" customHeight="1">
       <c r="A36" s="42" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="B36" s="63" t="s">
         <v>38</v>
@@ -6606,7 +6606,7 @@
         <v>298</v>
       </c>
       <c r="E36" s="65" t="s">
-        <v>439</v>
+        <v>489</v>
       </c>
       <c r="F36" s="64" t="s">
         <v>78</v>
@@ -6618,7 +6618,7 @@
         <v>414</v>
       </c>
       <c r="I36" s="197" t="s">
-        <v>415</v>
+        <v>19</v>
       </c>
       <c r="J36" s="63" t="s">
         <v>95</v>
@@ -6657,7 +6657,7 @@
     </row>
     <row r="37" spans="1:29" s="171" customFormat="1" ht="25" customHeight="1">
       <c r="A37" s="42" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B37" s="63" t="s">
         <v>38</v>
@@ -6669,7 +6669,7 @@
         <v>422</v>
       </c>
       <c r="E37" s="65" t="s">
-        <v>439</v>
+        <v>489</v>
       </c>
       <c r="F37" s="64" t="s">
         <v>78</v>
@@ -6681,7 +6681,7 @@
         <v>414</v>
       </c>
       <c r="I37" s="197" t="s">
-        <v>415</v>
+        <v>19</v>
       </c>
       <c r="J37" s="63" t="s">
         <v>95</v>
@@ -6720,7 +6720,7 @@
     </row>
     <row r="38" spans="1:29" s="171" customFormat="1" ht="25" customHeight="1">
       <c r="A38" s="42" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B38" s="63" t="s">
         <v>38</v>
@@ -6732,7 +6732,7 @@
         <v>252</v>
       </c>
       <c r="E38" s="65" t="s">
-        <v>439</v>
+        <v>489</v>
       </c>
       <c r="F38" s="64" t="s">
         <v>78</v>
@@ -6744,7 +6744,7 @@
         <v>414</v>
       </c>
       <c r="I38" s="197" t="s">
-        <v>415</v>
+        <v>19</v>
       </c>
       <c r="J38" s="63" t="s">
         <v>95</v>
@@ -6783,7 +6783,7 @@
     </row>
     <row r="39" spans="1:29" ht="25" customHeight="1">
       <c r="A39" s="42" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="B39" s="63" t="s">
         <v>38</v>
@@ -6795,7 +6795,7 @@
         <v>253</v>
       </c>
       <c r="E39" s="65" t="s">
-        <v>439</v>
+        <v>489</v>
       </c>
       <c r="F39" s="64" t="s">
         <v>78</v>
@@ -6807,7 +6807,7 @@
         <v>414</v>
       </c>
       <c r="I39" s="197" t="s">
-        <v>415</v>
+        <v>19</v>
       </c>
       <c r="J39" s="63" t="s">
         <v>95</v>
@@ -6846,7 +6846,7 @@
     </row>
     <row r="40" spans="1:29" ht="25" customHeight="1">
       <c r="A40" s="42" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="B40" s="63" t="s">
         <v>38</v>
@@ -6858,7 +6858,7 @@
         <v>254</v>
       </c>
       <c r="E40" s="65" t="s">
-        <v>439</v>
+        <v>489</v>
       </c>
       <c r="F40" s="64" t="s">
         <v>78</v>
@@ -6870,7 +6870,7 @@
         <v>414</v>
       </c>
       <c r="I40" s="197" t="s">
-        <v>415</v>
+        <v>19</v>
       </c>
       <c r="J40" s="63" t="s">
         <v>95</v>
@@ -6909,7 +6909,7 @@
     </row>
     <row r="41" spans="1:29" ht="25" customHeight="1">
       <c r="A41" s="42" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="B41" s="63" t="s">
         <v>38</v>
@@ -6921,7 +6921,7 @@
         <v>423</v>
       </c>
       <c r="E41" s="65" t="s">
-        <v>439</v>
+        <v>489</v>
       </c>
       <c r="F41" s="64" t="s">
         <v>78</v>
@@ -6933,7 +6933,7 @@
         <v>414</v>
       </c>
       <c r="I41" s="197" t="s">
-        <v>415</v>
+        <v>19</v>
       </c>
       <c r="J41" s="63" t="s">
         <v>95</v>
@@ -6972,7 +6972,7 @@
     </row>
     <row r="42" spans="1:29" ht="25" customHeight="1">
       <c r="A42" s="42" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B42" s="63" t="s">
         <v>38</v>
@@ -6984,7 +6984,7 @@
         <v>424</v>
       </c>
       <c r="E42" s="65" t="s">
-        <v>439</v>
+        <v>489</v>
       </c>
       <c r="F42" s="64" t="s">
         <v>78</v>
@@ -6996,7 +6996,7 @@
         <v>414</v>
       </c>
       <c r="I42" s="197" t="s">
-        <v>415</v>
+        <v>19</v>
       </c>
       <c r="J42" s="63" t="s">
         <v>95</v>
@@ -7035,7 +7035,7 @@
     </row>
     <row r="43" spans="1:29" ht="25" customHeight="1">
       <c r="A43" s="42" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B43" s="63" t="s">
         <v>38</v>
@@ -7044,10 +7044,10 @@
         <v>410</v>
       </c>
       <c r="D43" s="32" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E43" s="65" t="s">
-        <v>439</v>
+        <v>489</v>
       </c>
       <c r="F43" s="64" t="s">
         <v>78</v>
@@ -7059,7 +7059,7 @@
         <v>414</v>
       </c>
       <c r="I43" s="197" t="s">
-        <v>415</v>
+        <v>19</v>
       </c>
       <c r="J43" s="63" t="s">
         <v>95</v>
@@ -7098,7 +7098,7 @@
     </row>
     <row r="44" spans="1:29" ht="25" customHeight="1">
       <c r="A44" s="42" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="B44" s="63" t="s">
         <v>38</v>
@@ -7107,10 +7107,10 @@
         <v>410</v>
       </c>
       <c r="D44" s="32" t="s">
-        <v>256</v>
+        <v>425</v>
       </c>
       <c r="E44" s="65" t="s">
-        <v>439</v>
+        <v>489</v>
       </c>
       <c r="F44" s="64" t="s">
         <v>78</v>
@@ -7122,7 +7122,7 @@
         <v>414</v>
       </c>
       <c r="I44" s="197" t="s">
-        <v>415</v>
+        <v>19</v>
       </c>
       <c r="J44" s="63" t="s">
         <v>95</v>
@@ -7161,7 +7161,7 @@
     </row>
     <row r="45" spans="1:29" ht="25" customHeight="1">
       <c r="A45" s="42" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="B45" s="63" t="s">
         <v>38</v>
@@ -7170,10 +7170,10 @@
         <v>410</v>
       </c>
       <c r="D45" s="32" t="s">
-        <v>257</v>
+        <v>321</v>
       </c>
       <c r="E45" s="65" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="F45" s="64" t="s">
         <v>78</v>
@@ -7185,7 +7185,7 @@
         <v>414</v>
       </c>
       <c r="I45" s="197" t="s">
-        <v>415</v>
+        <v>104</v>
       </c>
       <c r="J45" s="63" t="s">
         <v>95</v>
@@ -7224,7 +7224,7 @@
     </row>
     <row r="46" spans="1:29" ht="25" customHeight="1">
       <c r="A46" s="42" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="B46" s="63" t="s">
         <v>38</v>
@@ -7233,10 +7233,10 @@
         <v>410</v>
       </c>
       <c r="D46" s="32" t="s">
-        <v>425</v>
+        <v>322</v>
       </c>
       <c r="E46" s="65" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="F46" s="64" t="s">
         <v>78</v>
@@ -7248,7 +7248,7 @@
         <v>414</v>
       </c>
       <c r="I46" s="197" t="s">
-        <v>415</v>
+        <v>104</v>
       </c>
       <c r="J46" s="63" t="s">
         <v>95</v>
@@ -7287,7 +7287,7 @@
     </row>
     <row r="47" spans="1:29" ht="25" customHeight="1">
       <c r="A47" s="42" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B47" s="63" t="s">
         <v>38</v>
@@ -7296,10 +7296,10 @@
         <v>410</v>
       </c>
       <c r="D47" s="32" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E47" s="65" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="F47" s="64" t="s">
         <v>78</v>
@@ -7311,7 +7311,7 @@
         <v>414</v>
       </c>
       <c r="I47" s="197" t="s">
-        <v>415</v>
+        <v>104</v>
       </c>
       <c r="J47" s="63" t="s">
         <v>95</v>
@@ -7350,7 +7350,7 @@
     </row>
     <row r="48" spans="1:29" ht="25" customHeight="1">
       <c r="A48" s="42" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B48" s="63" t="s">
         <v>38</v>
@@ -7362,7 +7362,7 @@
         <v>322</v>
       </c>
       <c r="E48" s="65" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="F48" s="64" t="s">
         <v>78</v>
@@ -7374,7 +7374,7 @@
         <v>414</v>
       </c>
       <c r="I48" s="197" t="s">
-        <v>415</v>
+        <v>104</v>
       </c>
       <c r="J48" s="63" t="s">
         <v>95</v>
@@ -7413,7 +7413,7 @@
     </row>
     <row r="49" spans="1:29" ht="25" customHeight="1">
       <c r="A49" s="42" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="B49" s="63" t="s">
         <v>38</v>
@@ -7421,8 +7421,12 @@
       <c r="C49" s="64" t="s">
         <v>410</v>
       </c>
-      <c r="D49" s="64"/>
-      <c r="E49" s="65"/>
+      <c r="D49" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="E49" s="65" t="s">
+        <v>437</v>
+      </c>
       <c r="F49" s="64" t="s">
         <v>78</v>
       </c>
@@ -7433,7 +7437,7 @@
         <v>414</v>
       </c>
       <c r="I49" s="197" t="s">
-        <v>415</v>
+        <v>104</v>
       </c>
       <c r="J49" s="63" t="s">
         <v>95</v>
@@ -7472,7 +7476,7 @@
     </row>
     <row r="50" spans="1:29" s="173" customFormat="1" ht="25" customHeight="1">
       <c r="A50" s="42" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="B50" s="63" t="s">
         <v>38</v>
@@ -7480,8 +7484,12 @@
       <c r="C50" s="64" t="s">
         <v>410</v>
       </c>
-      <c r="D50" s="64"/>
-      <c r="E50" s="65"/>
+      <c r="D50" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="E50" s="65" t="s">
+        <v>437</v>
+      </c>
       <c r="F50" s="64" t="s">
         <v>78</v>
       </c>
@@ -7492,7 +7500,7 @@
         <v>414</v>
       </c>
       <c r="I50" s="197" t="s">
-        <v>415</v>
+        <v>104</v>
       </c>
       <c r="J50" s="63" t="s">
         <v>95</v>
@@ -7531,7 +7539,7 @@
     </row>
     <row r="51" spans="1:29" s="173" customFormat="1" ht="25" customHeight="1">
       <c r="A51" s="42" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B51" s="63" t="s">
         <v>38</v>
@@ -7539,8 +7547,12 @@
       <c r="C51" s="64" t="s">
         <v>410</v>
       </c>
-      <c r="D51" s="64"/>
-      <c r="E51" s="65"/>
+      <c r="D51" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="E51" s="65" t="s">
+        <v>437</v>
+      </c>
       <c r="F51" s="64" t="s">
         <v>78</v>
       </c>
@@ -7551,7 +7563,7 @@
         <v>414</v>
       </c>
       <c r="I51" s="197" t="s">
-        <v>415</v>
+        <v>104</v>
       </c>
       <c r="J51" s="63" t="s">
         <v>95</v>
@@ -7590,7 +7602,7 @@
     </row>
     <row r="52" spans="1:29" s="173" customFormat="1" ht="25" customHeight="1">
       <c r="A52" s="42" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="B52" s="63" t="s">
         <v>38</v>
@@ -7598,8 +7610,12 @@
       <c r="C52" s="64" t="s">
         <v>410</v>
       </c>
-      <c r="D52" s="64"/>
-      <c r="E52" s="65"/>
+      <c r="D52" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="E52" s="65" t="s">
+        <v>437</v>
+      </c>
       <c r="F52" s="64" t="s">
         <v>78</v>
       </c>
@@ -7610,7 +7626,7 @@
         <v>414</v>
       </c>
       <c r="I52" s="197" t="s">
-        <v>415</v>
+        <v>104</v>
       </c>
       <c r="J52" s="63" t="s">
         <v>95</v>
@@ -7649,7 +7665,7 @@
     </row>
     <row r="53" spans="1:29" s="173" customFormat="1" ht="25" customHeight="1">
       <c r="A53" s="42" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="B53" s="63" t="s">
         <v>38</v>
@@ -7657,8 +7673,12 @@
       <c r="C53" s="64" t="s">
         <v>410</v>
       </c>
-      <c r="D53" s="64"/>
-      <c r="E53" s="65"/>
+      <c r="D53" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="E53" s="65" t="s">
+        <v>437</v>
+      </c>
       <c r="F53" s="64" t="s">
         <v>78</v>
       </c>
@@ -7669,7 +7689,7 @@
         <v>414</v>
       </c>
       <c r="I53" s="197" t="s">
-        <v>415</v>
+        <v>104</v>
       </c>
       <c r="J53" s="63" t="s">
         <v>95</v>
@@ -7708,7 +7728,7 @@
     </row>
     <row r="54" spans="1:29" s="173" customFormat="1" ht="25" customHeight="1">
       <c r="A54" s="42" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="B54" s="63" t="s">
         <v>38</v>
@@ -7716,8 +7736,12 @@
       <c r="C54" s="64" t="s">
         <v>410</v>
       </c>
-      <c r="D54" s="64"/>
-      <c r="E54" s="65"/>
+      <c r="D54" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="E54" s="65" t="s">
+        <v>437</v>
+      </c>
       <c r="F54" s="64" t="s">
         <v>78</v>
       </c>
@@ -7728,7 +7752,7 @@
         <v>414</v>
       </c>
       <c r="I54" s="197" t="s">
-        <v>415</v>
+        <v>104</v>
       </c>
       <c r="J54" s="63" t="s">
         <v>95</v>
@@ -7767,7 +7791,7 @@
     </row>
     <row r="55" spans="1:29" s="173" customFormat="1" ht="25" customHeight="1">
       <c r="A55" s="42" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="B55" s="63" t="s">
         <v>38</v>
@@ -7775,8 +7799,12 @@
       <c r="C55" s="64" t="s">
         <v>410</v>
       </c>
-      <c r="D55" s="64"/>
-      <c r="E55" s="65"/>
+      <c r="D55" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="E55" s="65" t="s">
+        <v>437</v>
+      </c>
       <c r="F55" s="64" t="s">
         <v>78</v>
       </c>
@@ -7787,7 +7815,7 @@
         <v>414</v>
       </c>
       <c r="I55" s="197" t="s">
-        <v>415</v>
+        <v>104</v>
       </c>
       <c r="J55" s="63" t="s">
         <v>95</v>
@@ -7826,7 +7854,7 @@
     </row>
     <row r="56" spans="1:29" s="173" customFormat="1" ht="25" customHeight="1">
       <c r="A56" s="42" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="B56" s="63" t="s">
         <v>38</v>
@@ -7834,8 +7862,12 @@
       <c r="C56" s="64" t="s">
         <v>410</v>
       </c>
-      <c r="D56" s="64"/>
-      <c r="E56" s="65"/>
+      <c r="D56" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="E56" s="65" t="s">
+        <v>437</v>
+      </c>
       <c r="F56" s="64" t="s">
         <v>78</v>
       </c>
@@ -7846,7 +7878,7 @@
         <v>414</v>
       </c>
       <c r="I56" s="197" t="s">
-        <v>415</v>
+        <v>104</v>
       </c>
       <c r="J56" s="63" t="s">
         <v>95</v>
@@ -7885,7 +7917,7 @@
     </row>
     <row r="57" spans="1:29" s="173" customFormat="1" ht="25" customHeight="1">
       <c r="A57" s="42" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="B57" s="63" t="s">
         <v>38</v>
@@ -7893,8 +7925,12 @@
       <c r="C57" s="64" t="s">
         <v>410</v>
       </c>
-      <c r="D57" s="64"/>
-      <c r="E57" s="65"/>
+      <c r="D57" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="E57" s="65" t="s">
+        <v>437</v>
+      </c>
       <c r="F57" s="64" t="s">
         <v>78</v>
       </c>
@@ -7905,7 +7941,7 @@
         <v>414</v>
       </c>
       <c r="I57" s="197" t="s">
-        <v>415</v>
+        <v>104</v>
       </c>
       <c r="J57" s="63" t="s">
         <v>95</v>
@@ -7944,7 +7980,7 @@
     </row>
     <row r="58" spans="1:29" s="173" customFormat="1" ht="25" customHeight="1">
       <c r="A58" s="42" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="B58" s="63" t="s">
         <v>38</v>
@@ -7952,8 +7988,12 @@
       <c r="C58" s="64" t="s">
         <v>410</v>
       </c>
-      <c r="D58" s="64"/>
-      <c r="E58" s="65"/>
+      <c r="D58" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="E58" s="65" t="s">
+        <v>437</v>
+      </c>
       <c r="F58" s="64" t="s">
         <v>78</v>
       </c>
@@ -7964,7 +8004,7 @@
         <v>414</v>
       </c>
       <c r="I58" s="197" t="s">
-        <v>415</v>
+        <v>104</v>
       </c>
       <c r="J58" s="63" t="s">
         <v>95</v>
@@ -8003,7 +8043,7 @@
     </row>
     <row r="59" spans="1:29" s="173" customFormat="1" ht="25" customHeight="1">
       <c r="A59" s="42" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B59" s="63" t="s">
         <v>38</v>
@@ -8011,8 +8051,12 @@
       <c r="C59" s="64" t="s">
         <v>410</v>
       </c>
-      <c r="D59" s="64"/>
-      <c r="E59" s="65"/>
+      <c r="D59" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="E59" s="65" t="s">
+        <v>437</v>
+      </c>
       <c r="F59" s="64" t="s">
         <v>78</v>
       </c>
@@ -8023,7 +8067,7 @@
         <v>414</v>
       </c>
       <c r="I59" s="197" t="s">
-        <v>415</v>
+        <v>104</v>
       </c>
       <c r="J59" s="63" t="s">
         <v>95</v>
@@ -8062,7 +8106,7 @@
     </row>
     <row r="60" spans="1:29" s="173" customFormat="1" ht="25" customHeight="1">
       <c r="A60" s="42" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="B60" s="63" t="s">
         <v>38</v>
@@ -8070,8 +8114,12 @@
       <c r="C60" s="64" t="s">
         <v>410</v>
       </c>
-      <c r="D60" s="64"/>
-      <c r="E60" s="65"/>
+      <c r="D60" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="E60" s="65" t="s">
+        <v>437</v>
+      </c>
       <c r="F60" s="64" t="s">
         <v>78</v>
       </c>
@@ -8082,7 +8130,7 @@
         <v>414</v>
       </c>
       <c r="I60" s="197" t="s">
-        <v>415</v>
+        <v>104</v>
       </c>
       <c r="J60" s="63" t="s">
         <v>95</v>
@@ -8121,7 +8169,7 @@
     </row>
     <row r="61" spans="1:29" s="173" customFormat="1" ht="25" customHeight="1">
       <c r="A61" s="42" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="B61" s="63" t="s">
         <v>38</v>
@@ -8129,8 +8177,12 @@
       <c r="C61" s="64" t="s">
         <v>410</v>
       </c>
-      <c r="D61" s="64"/>
-      <c r="E61" s="65"/>
+      <c r="D61" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="E61" s="65" t="s">
+        <v>437</v>
+      </c>
       <c r="F61" s="64" t="s">
         <v>78</v>
       </c>
@@ -8141,7 +8193,7 @@
         <v>414</v>
       </c>
       <c r="I61" s="197" t="s">
-        <v>415</v>
+        <v>104</v>
       </c>
       <c r="J61" s="63" t="s">
         <v>95</v>
@@ -8180,7 +8232,7 @@
     </row>
     <row r="62" spans="1:29" s="173" customFormat="1" ht="25" customHeight="1">
       <c r="A62" s="42" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="B62" s="63" t="s">
         <v>38</v>
@@ -8188,8 +8240,12 @@
       <c r="C62" s="64" t="s">
         <v>410</v>
       </c>
-      <c r="D62" s="64"/>
-      <c r="E62" s="65"/>
+      <c r="D62" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="E62" s="65" t="s">
+        <v>437</v>
+      </c>
       <c r="F62" s="64" t="s">
         <v>78</v>
       </c>
@@ -8200,7 +8256,7 @@
         <v>414</v>
       </c>
       <c r="I62" s="197" t="s">
-        <v>415</v>
+        <v>104</v>
       </c>
       <c r="J62" s="63" t="s">
         <v>95</v>

</xml_diff>